<commit_message>
Push outputs from CI/CD (2026-02-19 10:48:54)
</commit_message>
<xml_diff>
--- a/production/watch-dk-PRELIMINARY/Manufacturing/Assembly/ZSWatch-Watch-DevKit-bom.xlsx
+++ b/production/watch-dk-PRELIMINARY/Manufacturing/Assembly/ZSWatch-Watch-DevKit-bom.xlsx
@@ -1094,7 +1094,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>9.0.6+1</t>
+    <t>9.0.7+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -1271,7 +1271,7 @@
     <t>Created:</t>
   </si>
   <si>
-    <t>2025-12-31 09:57:20</t>
+    <t>2026-02-19 10:55:35</t>
   </si>
   <si>
     <t>KiCost® v1.1.20 + KiBot v1.8.5</t>

</xml_diff>